<commit_message>
i am gonna sleep
</commit_message>
<xml_diff>
--- a/Attach/FactoryClient/FactoryClient/bin/Debug/菜單.xlsx
+++ b/Attach/FactoryClient/FactoryClient/bin/Debug/菜單.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDE1B7-48CE-4750-AFD6-ECF0669E2754}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E7CB88-5AED-456C-9856-EFBB3875F9A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3975" windowWidth="15630" windowHeight="7140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="112">
   <si>
     <t>編號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,6 +74,9 @@
     <t>台灣小吃部(1)</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:09</t>
+  </si>
+  <si>
     <t>海苔御飯糰</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
     <t>焗烤白醬麵+起司豬排</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:10</t>
+  </si>
+  <si>
     <t>熱狗蛋炒飯+雞排</t>
   </si>
   <si>
@@ -101,15 +107,39 @@
     <t>韓式拌飯</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:11</t>
+  </si>
+  <si>
     <t>牛肉粥</t>
   </si>
   <si>
     <t>皮蛋瘦肉粥</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:12</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:13</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:14</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:15</t>
+  </si>
+  <si>
     <t>閒置的餐點</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:16</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:17</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:18</t>
+  </si>
+  <si>
     <t>卡拉雞+三副菜</t>
   </si>
   <si>
@@ -119,241 +149,217 @@
     <t>起司豬排+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:19</t>
+  </si>
+  <si>
     <t>蒜泥白肉+三副菜</t>
   </si>
   <si>
     <t>烤肉飯+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:20</t>
+  </si>
+  <si>
     <t>香煎無骨雞腿排+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:21</t>
+  </si>
+  <si>
     <t>蒜香鹹豬肉+三副菜</t>
   </si>
   <si>
     <t>浦燒魚飯+雞塊+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:22</t>
+  </si>
+  <si>
     <t>鐵路豬排+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:23</t>
+  </si>
+  <si>
     <t>無骨雞排飯+三副菜</t>
   </si>
   <si>
     <t>雞腿飯+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:24</t>
+  </si>
+  <si>
     <t>黑胡椒豬柳+三副菜</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:25</t>
+  </si>
+  <si>
     <t>原味小火鍋</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:26</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:27</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:28</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:29</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:30</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:31</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:32</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:33</t>
+  </si>
+  <si>
     <t>張君雅泡乾麵+荷包蛋+青菜</t>
   </si>
   <si>
     <t>麵食部(3)</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:34</t>
+  </si>
+  <si>
     <t>台南擔仔乾麵+荷包蛋+小菜</t>
   </si>
   <si>
     <t>乾粄條+小菜+蛋</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:35</t>
+  </si>
+  <si>
     <t>牛肉湯麵</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:36</t>
+  </si>
+  <si>
     <t>酸辣湯餃</t>
   </si>
   <si>
     <t>味噌拉麵+蛋</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:37</t>
+  </si>
+  <si>
     <t>麻辣湯麵(張君雅)+豬血+臭豆腐</t>
   </si>
   <si>
     <t>牛肉麵</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:38</t>
+  </si>
+  <si>
     <t>沙茶羊肉羹麵</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:39</t>
+  </si>
+  <si>
     <t>麻辣湯張君雅+豬血+臭豆腐+肉片</t>
   </si>
   <si>
     <t>味噌拉麵+蛋+卡拉雞</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:40</t>
+  </si>
+  <si>
     <t>烤肉乾麵</t>
   </si>
   <si>
     <t>酸辣湯麵 蛋 雞腿</t>
   </si>
   <si>
+    <t>2019-06-18-19:30:41</t>
+  </si>
+  <si>
     <t>貢丸豚骨麵</t>
   </si>
   <si>
-    <t>2019-06-18-22:56:30</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:31</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:32</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:33</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:34</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:35</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:36</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:37</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:38</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:39</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:40</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:41</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:42</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:43</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:44</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:45</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:46</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:47</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:48</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:49</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:50</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:51</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:52</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:53</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:54</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:55</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:56</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:57</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:58</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:56:59</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:00</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:01</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:02</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:03</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:04</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:05</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:06</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:07</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:08</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:09</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:10</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:11</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:12</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:13</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:14</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:15</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:16</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:17</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:18</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:19</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:20</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:21</t>
-  </si>
-  <si>
-    <t>2019-06-18-22:57:22</t>
-  </si>
-  <si>
-    <t>蔥抓餅+蛋+雞排</t>
+    <t>2019-06-18-19:30:42</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:43</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:44</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:45</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:46</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:47</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:48</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:49</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:50</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:51</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:52</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:53</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:54</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:55</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:56</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:57</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:58</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:30:59</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:31:00</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:31:01</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:31:02</t>
+  </si>
+  <si>
+    <t>2019-06-18-19:31:03</t>
+  </si>
+  <si>
+    <t>蔥抓餅+蛋+雞排2333</t>
   </si>
 </sst>
 </file>
@@ -942,7 +948,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -987,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>40</v>
@@ -1008,7 +1014,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1016,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -1037,7 +1043,7 @@
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1045,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -1066,7 +1072,7 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1074,7 +1080,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -1095,7 +1101,7 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1103,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>40</v>
@@ -1124,7 +1130,7 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1132,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>55</v>
@@ -1153,7 +1159,7 @@
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1161,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>55</v>
@@ -1182,7 +1188,7 @@
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1190,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>55</v>
@@ -1211,7 +1217,7 @@
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1219,7 +1225,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>55</v>
@@ -1240,7 +1246,7 @@
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1248,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>55</v>
@@ -1269,7 +1275,7 @@
         <v>15</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1277,7 +1283,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>55</v>
@@ -1298,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1306,7 +1312,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>55</v>
@@ -1327,7 +1333,7 @@
         <v>15</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1335,7 +1341,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>55</v>
@@ -1356,7 +1362,7 @@
         <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1382,7 +1388,7 @@
         <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1408,7 +1414,7 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1434,7 +1440,7 @@
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1460,7 +1466,7 @@
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1486,7 +1492,7 @@
         <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1512,7 +1518,7 @@
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1538,7 +1544,7 @@
         <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1546,7 +1552,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C22">
         <v>123</v>
@@ -1567,7 +1573,7 @@
         <v>15</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1575,7 +1581,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>123</v>
@@ -1596,7 +1602,7 @@
         <v>15</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1604,7 +1610,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>123</v>
@@ -1625,7 +1631,7 @@
         <v>15</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1633,7 +1639,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <v>123</v>
@@ -1654,7 +1660,7 @@
         <v>15</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1662,7 +1668,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>123</v>
@@ -1683,7 +1689,7 @@
         <v>15</v>
       </c>
       <c r="I26" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1691,7 +1697,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C27">
         <v>55</v>
@@ -1706,13 +1712,13 @@
         <v>-1</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I27" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1720,7 +1726,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C28">
         <v>55</v>
@@ -1735,13 +1741,13 @@
         <v>-1</v>
       </c>
       <c r="G28" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1749,7 +1755,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C29">
         <v>55</v>
@@ -1764,13 +1770,13 @@
         <v>-1</v>
       </c>
       <c r="G29" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I29" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1778,7 +1784,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>55</v>
@@ -1793,13 +1799,13 @@
         <v>-1</v>
       </c>
       <c r="G30" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1807,7 +1813,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C31">
         <v>55</v>
@@ -1822,13 +1828,13 @@
         <v>-1</v>
       </c>
       <c r="G31" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I31" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1836,7 +1842,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>55</v>
@@ -1851,13 +1857,13 @@
         <v>-1</v>
       </c>
       <c r="G32" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I32" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1865,7 +1871,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C33">
         <v>55</v>
@@ -1880,13 +1886,13 @@
         <v>-1</v>
       </c>
       <c r="G33" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1894,7 +1900,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C34">
         <v>55</v>
@@ -1909,13 +1915,13 @@
         <v>-1</v>
       </c>
       <c r="G34" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I34" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1923,7 +1929,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C35">
         <v>55</v>
@@ -1938,13 +1944,13 @@
         <v>-1</v>
       </c>
       <c r="G35" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I35" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1952,7 +1958,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C36">
         <v>55</v>
@@ -1967,13 +1973,13 @@
         <v>-1</v>
       </c>
       <c r="G36" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I36" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1981,7 +1987,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C37">
         <v>55</v>
@@ -1996,13 +2002,13 @@
         <v>-1</v>
       </c>
       <c r="G37" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I37" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2010,7 +2016,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C38">
         <v>123</v>
@@ -2025,13 +2031,13 @@
         <v>-1</v>
       </c>
       <c r="G38" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I38" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2051,13 +2057,13 @@
         <v>-1</v>
       </c>
       <c r="G39" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I39" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2065,7 +2071,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C40">
         <v>123</v>
@@ -2080,13 +2086,13 @@
         <v>-1</v>
       </c>
       <c r="G40" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I40" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2094,7 +2100,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>123</v>
@@ -2109,13 +2115,13 @@
         <v>-1</v>
       </c>
       <c r="G41" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I41" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2123,7 +2129,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C42">
         <v>123</v>
@@ -2138,13 +2144,13 @@
         <v>-1</v>
       </c>
       <c r="G42" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I42" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2152,7 +2158,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C43">
         <v>123</v>
@@ -2167,13 +2173,13 @@
         <v>-1</v>
       </c>
       <c r="G43" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I43" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2181,7 +2187,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C44">
         <v>123</v>
@@ -2196,13 +2202,13 @@
         <v>-1</v>
       </c>
       <c r="G44" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I44" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2210,7 +2216,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C45">
         <v>123</v>
@@ -2225,13 +2231,13 @@
         <v>-1</v>
       </c>
       <c r="G45" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I45" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2239,7 +2245,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C46">
         <v>123</v>
@@ -2254,13 +2260,13 @@
         <v>-1</v>
       </c>
       <c r="G46" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I46" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2268,7 +2274,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C47">
         <v>123</v>
@@ -2283,13 +2289,13 @@
         <v>-1</v>
       </c>
       <c r="G47" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I47" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2297,7 +2303,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C48">
         <v>123</v>
@@ -2312,13 +2318,13 @@
         <v>-1</v>
       </c>
       <c r="G48" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2326,7 +2332,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C49">
         <v>123</v>
@@ -2341,13 +2347,13 @@
         <v>-1</v>
       </c>
       <c r="G49" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I49" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2355,7 +2361,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C50">
         <v>123</v>
@@ -2370,13 +2376,13 @@
         <v>-1</v>
       </c>
       <c r="G50" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I50" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2384,7 +2390,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C51">
         <v>123</v>
@@ -2399,13 +2405,13 @@
         <v>-1</v>
       </c>
       <c r="G51" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I51" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2413,7 +2419,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C52">
         <v>40</v>
@@ -2428,13 +2434,13 @@
         <v>-1</v>
       </c>
       <c r="G52" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2442,7 +2448,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C53">
         <v>40</v>
@@ -2457,13 +2463,13 @@
         <v>-1</v>
       </c>
       <c r="G53" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I53" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2471,7 +2477,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C54">
         <v>40</v>
@@ -2486,13 +2492,13 @@
         <v>-1</v>
       </c>
       <c r="G54" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I54" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2500,7 +2506,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C55">
         <v>40</v>
@@ -2515,13 +2521,13 @@
         <v>-1</v>
       </c>
       <c r="G55" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I55" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2529,7 +2535,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C56">
         <v>40</v>
@@ -2544,13 +2550,13 @@
         <v>-1</v>
       </c>
       <c r="G56" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I56" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2558,7 +2564,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C57">
         <v>40</v>
@@ -2573,13 +2579,13 @@
         <v>-1</v>
       </c>
       <c r="G57" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I57" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2587,7 +2593,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="C58">
         <v>40</v>
@@ -2602,13 +2608,13 @@
         <v>-1</v>
       </c>
       <c r="G58" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I58" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2616,7 +2622,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C59">
         <v>55</v>
@@ -2631,13 +2637,13 @@
         <v>-1</v>
       </c>
       <c r="G59" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I59" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2645,7 +2651,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C60">
         <v>55</v>
@@ -2660,13 +2666,13 @@
         <v>-1</v>
       </c>
       <c r="G60" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I60" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2674,7 +2680,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C61">
         <v>55</v>
@@ -2689,13 +2695,13 @@
         <v>-1</v>
       </c>
       <c r="G61" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I61" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2703,7 +2709,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C62">
         <v>55</v>
@@ -2718,13 +2724,13 @@
         <v>-1</v>
       </c>
       <c r="G62" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2732,7 +2738,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="C63">
         <v>55</v>
@@ -2747,13 +2753,13 @@
         <v>-1</v>
       </c>
       <c r="G63" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2761,7 +2767,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C64">
         <v>55</v>
@@ -2776,7 +2782,7 @@
         <v>-1</v>
       </c>
       <c r="G64" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>15</v>
@@ -2790,7 +2796,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C65">
         <v>55</v>
@@ -2805,13 +2811,13 @@
         <v>-1</v>
       </c>
       <c r="G65" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I65" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2831,13 +2837,13 @@
         <v>-1</v>
       </c>
       <c r="G66" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I66" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2857,13 +2863,13 @@
         <v>-1</v>
       </c>
       <c r="G67" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I67" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2871,7 +2877,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C68">
         <v>123</v>
@@ -2886,13 +2892,13 @@
         <v>-1</v>
       </c>
       <c r="G68" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I68" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2900,7 +2906,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C69">
         <v>123</v>
@@ -2915,13 +2921,13 @@
         <v>-1</v>
       </c>
       <c r="G69" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I69" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2929,7 +2935,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C70">
         <v>123</v>
@@ -2944,13 +2950,13 @@
         <v>-1</v>
       </c>
       <c r="G70" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I70" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2958,7 +2964,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C71">
         <v>123</v>
@@ -2973,13 +2979,13 @@
         <v>-1</v>
       </c>
       <c r="G71" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I71" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2987,7 +2993,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C72">
         <v>123</v>
@@ -3002,13 +3008,13 @@
         <v>-1</v>
       </c>
       <c r="G72" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I72" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3016,7 +3022,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C73">
         <v>123</v>
@@ -3031,13 +3037,13 @@
         <v>-1</v>
       </c>
       <c r="G73" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3045,7 +3051,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C74">
         <v>123</v>
@@ -3060,13 +3066,13 @@
         <v>-1</v>
       </c>
       <c r="G74" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I74" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3074,7 +3080,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C75">
         <v>123</v>
@@ -3089,13 +3095,13 @@
         <v>-1</v>
       </c>
       <c r="G75" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I75" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3103,7 +3109,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C76">
         <v>123</v>
@@ -3118,13 +3124,13 @@
         <v>-1</v>
       </c>
       <c r="G76" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I76" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3132,7 +3138,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C77">
         <v>123</v>
@@ -3153,7 +3159,7 @@
         <v>15</v>
       </c>
       <c r="I77" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3161,7 +3167,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C78">
         <v>123</v>
@@ -3182,7 +3188,7 @@
         <v>15</v>
       </c>
       <c r="I78" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3190,7 +3196,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C79">
         <v>123</v>
@@ -3211,7 +3217,7 @@
         <v>15</v>
       </c>
       <c r="I79" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3219,7 +3225,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C80">
         <v>123</v>
@@ -3240,7 +3246,7 @@
         <v>15</v>
       </c>
       <c r="I80" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3248,7 +3254,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C81">
         <v>123</v>
@@ -3269,7 +3275,7 @@
         <v>15</v>
       </c>
       <c r="I81" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3277,7 +3283,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C82">
         <v>123</v>
@@ -3298,7 +3304,7 @@
         <v>15</v>
       </c>
       <c r="I82" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3306,7 +3312,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C83">
         <v>123</v>
@@ -3327,7 +3333,7 @@
         <v>15</v>
       </c>
       <c r="I83" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3335,7 +3341,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C84">
         <v>123</v>
@@ -3356,7 +3362,7 @@
         <v>15</v>
       </c>
       <c r="I84" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3364,7 +3370,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C85">
         <v>123</v>
@@ -3385,7 +3391,7 @@
         <v>15</v>
       </c>
       <c r="I85" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3393,7 +3399,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C86">
         <v>123</v>
@@ -3414,7 +3420,7 @@
         <v>15</v>
       </c>
       <c r="I86" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3422,7 +3428,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C87">
         <v>123</v>
@@ -3443,7 +3449,7 @@
         <v>15</v>
       </c>
       <c r="I87" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3451,7 +3457,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C88">
         <v>123</v>
@@ -3472,7 +3478,7 @@
         <v>15</v>
       </c>
       <c r="I88" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3480,7 +3486,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C89">
         <v>123</v>
@@ -3501,7 +3507,7 @@
         <v>15</v>
       </c>
       <c r="I89" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3509,7 +3515,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C90">
         <v>123</v>
@@ -3530,7 +3536,7 @@
         <v>15</v>
       </c>
       <c r="I90" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3538,7 +3544,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C91">
         <v>123</v>
@@ -3559,7 +3565,7 @@
         <v>15</v>
       </c>
       <c r="I91" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3567,7 +3573,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C92">
         <v>123</v>
@@ -3588,7 +3594,7 @@
         <v>15</v>
       </c>
       <c r="I92" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3596,7 +3602,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C93">
         <v>123</v>
@@ -3617,7 +3623,7 @@
         <v>15</v>
       </c>
       <c r="I93" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3625,7 +3631,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C94">
         <v>123</v>
@@ -3646,7 +3652,7 @@
         <v>15</v>
       </c>
       <c r="I94" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3654,7 +3660,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C95">
         <v>123</v>
@@ -3675,7 +3681,7 @@
         <v>15</v>
       </c>
       <c r="I95" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3683,7 +3689,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C96">
         <v>123</v>
@@ -3704,7 +3710,7 @@
         <v>15</v>
       </c>
       <c r="I96" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3712,7 +3718,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C97">
         <v>123</v>
@@ -3733,7 +3739,7 @@
         <v>15</v>
       </c>
       <c r="I97" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -3741,7 +3747,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C98">
         <v>123</v>
@@ -3762,7 +3768,7 @@
         <v>15</v>
       </c>
       <c r="I98" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3770,7 +3776,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C99">
         <v>123</v>
@@ -3791,7 +3797,7 @@
         <v>15</v>
       </c>
       <c r="I99" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -3799,7 +3805,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C100">
         <v>123</v>
@@ -3820,7 +3826,7 @@
         <v>15</v>
       </c>
       <c r="I100" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -3828,7 +3834,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C101">
         <v>123</v>
@@ -3849,7 +3855,7 @@
         <v>15</v>
       </c>
       <c r="I101" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>